<commit_message>
vault backup: 2023-02-06 11:58:47
</commit_message>
<xml_diff>
--- a/topic-12/output.xlsx
+++ b/topic-12/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -34,25 +34,13 @@
     <t>Preis</t>
   </si>
   <si>
-    <t>Tisch</t>
-  </si>
-  <si>
-    <t>34234</t>
-  </si>
-  <si>
-    <t>2342</t>
-  </si>
-  <si>
-    <t>Stuhl</t>
-  </si>
-  <si>
-    <t>234234</t>
-  </si>
-  <si>
-    <t>Monitor</t>
-  </si>
-  <si>
-    <t>234</t>
+    <t>tet</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
 </sst>
 </file>
@@ -384,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,50 +412,10 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>23434</v>
-      </c>
-      <c r="F4">
-        <v>234</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>